<commit_message>
update custom sort order
</commit_message>
<xml_diff>
--- a/data/custom sort order by job position.xlsx
+++ b/data/custom sort order by job position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chula-my.sharepoint.com/personal/prasert_k_chula_ac_th/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{89003FC5-BD46-4765-AFD3-71F0D6A6A2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C8D385-CA5B-4F48-93E0-ABFA7871040A}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{89003FC5-BD46-4765-AFD3-71F0D6A6A2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72CE59C8-E712-4E2B-B8B8-DCB1DBDD495F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="226" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" tabRatio="226" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employee" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>M</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>Sort Order</t>
+  </si>
+  <si>
+    <t>ฟ้า</t>
+  </si>
+  <si>
+    <t>อิงฟ้า</t>
+  </si>
+  <si>
+    <t>สายฟ้า</t>
+  </si>
+  <si>
+    <t>สายรุ้ง</t>
   </si>
 </sst>
 </file>
@@ -159,10 +171,10 @@
     <numFmt numFmtId="173" formatCode="[$-1070000]d\ mmm\ yyyy_);@_)"/>
     <numFmt numFmtId="174" formatCode="[$-D07041E]#,##0.00_);@_)"/>
     <numFmt numFmtId="175" formatCode="General_)"/>
-    <numFmt numFmtId="179" formatCode="#,##0_);[Red]\-#,##0_)"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00_);[Red]\-#,##0.00_)"/>
-    <numFmt numFmtId="181" formatCode="[$-409]d\-mmm\-yy_);@_)"/>
-    <numFmt numFmtId="184" formatCode="[$-409]dd\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="#,##0_);[Red]\-#,##0_)"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_);[Red]\-#,##0.00_)"/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm\-yy_);@_)"/>
+    <numFmt numFmtId="179" formatCode="[$-409]dd\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -377,8 +389,8 @@
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -394,17 +406,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="181" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="175" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="22"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="172" fontId="11" fillId="0" borderId="3" xfId="17" applyFont="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Calculation" xfId="2" builtinId="22" customBuiltin="1"/>
@@ -743,19 +755,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
@@ -768,14 +780,14 @@
       <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -788,14 +800,14 @@
       <c r="C2" s="4">
         <v>26416</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4">
+        <v>35723</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>101500</v>
-      </c>
-      <c r="F2" s="4">
-        <v>37193</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -808,14 +820,14 @@
       <c r="C3" s="4">
         <v>23886</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4">
+        <v>38894</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>54000</v>
-      </c>
-      <c r="F3" s="4">
-        <v>38894</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -828,14 +840,14 @@
       <c r="C4" s="4">
         <v>24074</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4">
+        <v>38124</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>72000</v>
-      </c>
-      <c r="F4" s="4">
-        <v>38124</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -846,16 +858,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>22123</v>
-      </c>
-      <c r="D5" t="s">
+        <v>32350</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42702</v>
+      </c>
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>31000</v>
-      </c>
-      <c r="F5" s="4">
-        <v>39049</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -868,14 +880,14 @@
       <c r="C6" s="4">
         <v>23042</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4">
+        <v>38459</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>50500</v>
-      </c>
-      <c r="F6" s="4">
-        <v>38459</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -888,14 +900,14 @@
       <c r="C7" s="4">
         <v>25904</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4">
+        <v>39256</v>
+      </c>
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>120000</v>
-      </c>
-      <c r="F7" s="4">
-        <v>39256</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -908,14 +920,14 @@
       <c r="C8" s="4">
         <v>22635</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4">
+        <v>37891</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>75000</v>
-      </c>
-      <c r="F8" s="4">
-        <v>37891</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -928,14 +940,14 @@
       <c r="C9" s="4">
         <v>27508</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4">
+        <v>36813</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>100000</v>
-      </c>
-      <c r="F9" s="4">
-        <v>36813</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -946,16 +958,16 @@
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>32274</v>
-      </c>
-      <c r="D10" t="s">
+        <v>35926</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42072</v>
+      </c>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>18500</v>
-      </c>
-      <c r="F10" s="4">
-        <v>42072</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -968,14 +980,14 @@
       <c r="C11" s="4">
         <v>33138</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4">
+        <v>42489</v>
+      </c>
+      <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>19000</v>
-      </c>
-      <c r="F11" s="4">
-        <v>42489</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -988,14 +1000,14 @@
       <c r="C12" s="4">
         <v>28723</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4">
+        <v>39343</v>
+      </c>
+      <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>82500</v>
-      </c>
-      <c r="F12" s="4">
-        <v>39343</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1008,14 +1020,14 @@
       <c r="C13" s="4">
         <v>26432</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4">
+        <v>38054</v>
+      </c>
+      <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>77500</v>
-      </c>
-      <c r="F13" s="4">
-        <v>38054</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1026,16 +1038,16 @@
         <v>2</v>
       </c>
       <c r="C14" s="4">
-        <v>26293</v>
-      </c>
-      <c r="D14" t="s">
+        <v>33598</v>
+      </c>
+      <c r="D14" s="4">
+        <v>41314</v>
+      </c>
+      <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>35000</v>
-      </c>
-      <c r="F14" s="4">
-        <v>37661</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1048,14 +1060,14 @@
       <c r="C15" s="4">
         <v>22559</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4">
+        <v>39861</v>
+      </c>
+      <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="2">
-        <v>24000</v>
-      </c>
-      <c r="F15" s="4">
-        <v>39861</v>
+      <c r="F15" s="2">
+        <v>22000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1068,14 +1080,14 @@
       <c r="C16" s="4">
         <v>24970</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4">
+        <v>38066</v>
+      </c>
+      <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>73000</v>
-      </c>
-      <c r="F16" s="4">
-        <v>38066</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1088,14 +1100,14 @@
       <c r="C17" s="4">
         <v>36635</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4">
+        <v>45031</v>
+      </c>
+      <c r="E17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>23500</v>
-      </c>
-      <c r="F17" s="4">
-        <v>45031</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1108,14 +1120,14 @@
       <c r="C18" s="4">
         <v>34630</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4">
+        <v>43861</v>
+      </c>
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>36500</v>
-      </c>
-      <c r="F18" s="4">
-        <v>43861</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1128,14 +1140,14 @@
       <c r="C19" s="4">
         <v>31446</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4">
+        <v>38425</v>
+      </c>
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>74000</v>
-      </c>
-      <c r="F19" s="4">
-        <v>38425</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1148,14 +1160,14 @@
       <c r="C20" s="4">
         <v>30522</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4">
+        <v>38038</v>
+      </c>
+      <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="2">
-        <v>74000</v>
-      </c>
-      <c r="F20" s="4">
-        <v>38038</v>
+      <c r="F20" s="2">
+        <v>77000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1168,14 +1180,94 @@
       <c r="C21" s="4">
         <v>26168</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2">
-        <v>87000</v>
-      </c>
-      <c r="F21" s="4">
-        <v>38176</v>
+      <c r="D21" s="4">
+        <v>36349</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>38222</v>
+      </c>
+      <c r="D22" s="4">
+        <v>45047</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2">
+        <v>18500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>37869</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45078</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="2">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>37655</v>
+      </c>
+      <c r="D24" s="4">
+        <v>45108</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="2">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>37389</v>
+      </c>
+      <c r="D25" s="4">
+        <v>45139</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="2">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>